<commit_message>
Split original data into training and testing files (11k Mark)
</commit_message>
<xml_diff>
--- a/src/Gabriel/Deliverable/Classification Ranking.xlsx
+++ b/src/Gabriel/Deliverable/Classification Ranking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="93">
   <si>
     <t>Accuracy</t>
   </si>
@@ -257,13 +257,52 @@
   </si>
   <si>
     <t>MinMax</t>
+  </si>
+  <si>
+    <t>SVC(C=3, cache_size=200, class_weight=None, coef0=0.0,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  decision_function_shape='ovr', degree=0.5, gamma=110, kernel='rbf',</t>
+  </si>
+  <si>
+    <t>{'C': 3, 'degree': 0.5, 'gamma': 110}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  decision_function_shape='ovr', degree=0.3, gamma=110, kernel='rbf',</t>
+  </si>
+  <si>
+    <t>{'C': 3, 'degree': 0.3, 'gamma': 110}</t>
+  </si>
+  <si>
+    <t>CV Split</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  decision_function_shape='ovr', degree=1, gamma=110, kernel='rbf',</t>
+  </si>
+  <si>
+    <t>60/40%</t>
+  </si>
+  <si>
+    <t>50/50%</t>
+  </si>
+  <si>
+    <t>var9(t), var4(t)</t>
+  </si>
+  <si>
+    <t>var(6)</t>
+  </si>
+  <si>
+    <t>var6(t), var2(t)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  decision_function_shape='ovr', degree=2, gamma=110, kernel='rbf',</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +317,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF008080"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -300,10 +345,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,11 +665,11 @@
     <col min="2" max="2" width="74.7109375" customWidth="1"/>
     <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -629,7 +677,7 @@
         <v>14980</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -637,7 +685,7 @@
         <v>14976</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -645,7 +693,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -662,16 +710,19 @@
         <v>58</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="H5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -688,56 +739,59 @@
         <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -754,56 +808,59 @@
         <v>78</v>
       </c>
       <c r="F15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="2">
+        <v>69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -820,60 +877,63 @@
         <v>78</v>
       </c>
       <c r="F24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" t="s">
         <v>1</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -890,56 +950,59 @@
         <v>78</v>
       </c>
       <c r="F33" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" t="s">
         <v>38</v>
       </c>
-      <c r="G33" s="2">
+      <c r="H33" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="H33" s="2">
+      <c r="I33" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -956,56 +1019,59 @@
         <v>78</v>
       </c>
       <c r="F42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" t="s">
         <v>47</v>
       </c>
-      <c r="G42" s="2">
+      <c r="H42" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -1022,28 +1088,520 @@
         <v>79</v>
       </c>
       <c r="F51" t="s">
-        <v>3</v>
-      </c>
-      <c r="G51" s="2">
+        <v>69</v>
+      </c>
+      <c r="G51" t="s">
+        <v>3</v>
+      </c>
+      <c r="H51" s="2">
         <v>0.94692923898500003</v>
       </c>
-      <c r="H51" s="2">
+      <c r="I51" s="2">
         <v>0.94672701896199996</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>79</v>
+      </c>
+      <c r="F55" t="s">
+        <v>69</v>
+      </c>
+      <c r="G55" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0.94726301735600005</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0.947075087501</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>80</v>
+      </c>
+      <c r="C59" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
+        <v>79</v>
+      </c>
+      <c r="F59" t="s">
+        <v>69</v>
+      </c>
+      <c r="G59" t="s">
+        <v>3</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.94726301735600005</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0.947075087501</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>9</v>
+      </c>
+      <c r="B63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63" t="s">
+        <v>79</v>
+      </c>
+      <c r="F63" t="s">
+        <v>70</v>
+      </c>
+      <c r="G63" t="s">
+        <v>3</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0.95704429112</v>
+      </c>
+      <c r="I63" s="2">
+        <v>0.95694260703</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>79</v>
+      </c>
+      <c r="F67" t="s">
+        <v>87</v>
+      </c>
+      <c r="G67" t="s">
+        <v>3</v>
+      </c>
+      <c r="H67" s="2">
+        <v>0.95710232014700003</v>
+      </c>
+      <c r="I67" s="2">
+        <v>0.956985178785</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>11</v>
+      </c>
+      <c r="B71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>79</v>
+      </c>
+      <c r="F71" t="s">
+        <v>88</v>
+      </c>
+      <c r="G71" t="s">
+        <v>3</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0.94845085470099999</v>
+      </c>
+      <c r="I71" s="2">
+        <v>0.948387035441</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>12</v>
+      </c>
+      <c r="B75" t="s">
+        <v>80</v>
+      </c>
+      <c r="C75" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>79</v>
+      </c>
+      <c r="F75" t="s">
+        <v>87</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H75" s="2">
+        <v>0.95576698380900005</v>
+      </c>
+      <c r="I75" s="2">
+        <v>0.95561167305100003</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>76</v>
+      </c>
+      <c r="C78" t="s">
+        <v>3</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>79</v>
+      </c>
+      <c r="F78" t="s">
+        <v>87</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H78" s="2">
+        <v>0.94658654648600005</v>
+      </c>
+      <c r="I78" s="2">
+        <v>0.94636419618400003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>13</v>
+      </c>
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>14</v>
+      </c>
+      <c r="B83" t="s">
+        <v>80</v>
+      </c>
+      <c r="C83" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>79</v>
+      </c>
+      <c r="F83" t="s">
+        <v>87</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H83" s="2">
+        <v>0.94858955099300002</v>
+      </c>
+      <c r="I83" s="2">
+        <v>0.94837828856600004</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>15</v>
+      </c>
+      <c r="B87" t="s">
+        <v>80</v>
+      </c>
+      <c r="C87" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>79</v>
+      </c>
+      <c r="F87" t="s">
+        <v>87</v>
+      </c>
+      <c r="G87" t="s">
+        <v>90</v>
+      </c>
+      <c r="H87" s="2">
+        <v>0.95543314972500004</v>
+      </c>
+      <c r="I87" s="2">
+        <v>0.95534929330200002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>16</v>
+      </c>
+      <c r="B91" t="s">
+        <v>80</v>
+      </c>
+      <c r="C91" t="s">
+        <v>3</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91" t="s">
+        <v>79</v>
+      </c>
+      <c r="F91" t="s">
+        <v>87</v>
+      </c>
+      <c r="G91" t="s">
+        <v>91</v>
+      </c>
+      <c r="H91" s="2">
+        <v>0.92889334001000001</v>
+      </c>
+      <c r="I91" s="2">
+        <v>0.92868399047799999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>17</v>
+      </c>
+      <c r="B95" t="s">
+        <v>80</v>
+      </c>
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>79</v>
+      </c>
+      <c r="F95" t="s">
+        <v>87</v>
+      </c>
+      <c r="G95" t="s">
+        <v>3</v>
+      </c>
+      <c r="H95" s="2">
+        <v>0.90233722871499999</v>
+      </c>
+      <c r="I95" s="2">
+        <v>0.90060578603599994</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1583,7 +2141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K156"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Testing on the test sample
</commit_message>
<xml_diff>
--- a/src/Gabriel/Deliverable/Classification Ranking.xlsx
+++ b/src/Gabriel/Deliverable/Classification Ranking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="106">
   <si>
     <t>Accuracy</t>
   </si>
@@ -296,6 +296,45 @@
   </si>
   <si>
     <t xml:space="preserve">  decision_function_shape='ovr', degree=2, gamma=110, kernel='rbf',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  decision_function_shape='ovr', degree=3, gamma=25, kernel='rbf',</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Prior Test File Splitting</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>60/40</t>
+  </si>
+  <si>
+    <t>{'C': 4, 'gamma': 25}</t>
+  </si>
+  <si>
+    <t>SVC(C=4, cache_size=200, class_weight=None, coef0=0.0,</t>
+  </si>
+  <si>
+    <t>70/30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  decision_function_shape='ovr', degree=3, gamma=35, kernel='rbf',</t>
+  </si>
+  <si>
+    <t>{'C': 2, 'gamma': 35}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  decision_function_shape='ovr', degree=3, gamma=30, kernel='rbf',</t>
+  </si>
+  <si>
+    <t>{'C': 3, 'gamma': 30}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            min_weight_fraction_leaf=0.0, n_estimators=10000, n_jobs=6,</t>
   </si>
 </sst>
 </file>
@@ -653,9 +692,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B82" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
@@ -665,11 +704,11 @@
     <col min="2" max="2" width="74.7109375" customWidth="1"/>
     <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="5" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -677,7 +716,7 @@
         <v>14980</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -685,7 +724,7 @@
         <v>14976</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -693,7 +732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -710,19 +749,22 @@
         <v>58</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="I5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -739,59 +781,62 @@
         <v>78</v>
       </c>
       <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
         <v>69</v>
       </c>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="H6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -808,59 +853,62 @@
         <v>78</v>
       </c>
       <c r="F15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" t="s">
         <v>69</v>
       </c>
-      <c r="G15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -877,63 +925,66 @@
         <v>78</v>
       </c>
       <c r="F24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G24" t="s">
         <v>69</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -950,59 +1001,62 @@
         <v>78</v>
       </c>
       <c r="F33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" t="s">
         <v>69</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>38</v>
       </c>
-      <c r="H33" s="2">
+      <c r="I33" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1019,59 +1073,62 @@
         <v>78</v>
       </c>
       <c r="F42" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" t="s">
         <v>69</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>47</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>0.54038718291099996</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>0.37914923039300003</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -1088,34 +1145,37 @@
         <v>79</v>
       </c>
       <c r="F51" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" t="s">
         <v>69</v>
       </c>
-      <c r="G51" t="s">
-        <v>3</v>
-      </c>
-      <c r="H51" s="2">
+      <c r="H51" t="s">
+        <v>3</v>
+      </c>
+      <c r="I51" s="2">
         <v>0.94692923898500003</v>
       </c>
-      <c r="I51" s="2">
+      <c r="J51" s="2">
         <v>0.94672701896199996</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7</v>
       </c>
@@ -1132,34 +1192,37 @@
         <v>79</v>
       </c>
       <c r="F55" t="s">
+        <v>96</v>
+      </c>
+      <c r="G55" t="s">
         <v>69</v>
       </c>
-      <c r="G55" t="s">
-        <v>3</v>
-      </c>
-      <c r="H55" s="2">
+      <c r="H55" t="s">
+        <v>3</v>
+      </c>
+      <c r="I55" s="2">
         <v>0.94726301735600005</v>
       </c>
-      <c r="I55" s="2">
+      <c r="J55" s="2">
         <v>0.947075087501</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8</v>
       </c>
@@ -1176,34 +1239,37 @@
         <v>79</v>
       </c>
       <c r="F59" t="s">
+        <v>96</v>
+      </c>
+      <c r="G59" t="s">
         <v>69</v>
       </c>
-      <c r="G59" t="s">
-        <v>3</v>
-      </c>
-      <c r="H59" s="2">
+      <c r="H59" t="s">
+        <v>3</v>
+      </c>
+      <c r="I59" s="2">
         <v>0.94726301735600005</v>
       </c>
-      <c r="I59" s="2">
+      <c r="J59" s="2">
         <v>0.947075087501</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9</v>
       </c>
@@ -1220,34 +1286,37 @@
         <v>79</v>
       </c>
       <c r="F63" t="s">
+        <v>96</v>
+      </c>
+      <c r="G63" t="s">
         <v>70</v>
       </c>
-      <c r="G63" t="s">
-        <v>3</v>
-      </c>
-      <c r="H63" s="2">
+      <c r="H63" t="s">
+        <v>3</v>
+      </c>
+      <c r="I63" s="2">
         <v>0.95704429112</v>
       </c>
-      <c r="I63" s="2">
+      <c r="J63" s="2">
         <v>0.95694260703</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>10</v>
       </c>
@@ -1264,34 +1333,37 @@
         <v>79</v>
       </c>
       <c r="F67" t="s">
+        <v>96</v>
+      </c>
+      <c r="G67" t="s">
         <v>87</v>
       </c>
-      <c r="G67" t="s">
-        <v>3</v>
-      </c>
-      <c r="H67" s="2">
+      <c r="H67" t="s">
+        <v>3</v>
+      </c>
+      <c r="I67" s="2">
         <v>0.95710232014700003</v>
       </c>
-      <c r="I67" s="2">
+      <c r="J67" s="2">
         <v>0.956985178785</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>11</v>
       </c>
@@ -1308,34 +1380,37 @@
         <v>79</v>
       </c>
       <c r="F71" t="s">
+        <v>96</v>
+      </c>
+      <c r="G71" t="s">
         <v>88</v>
       </c>
-      <c r="G71" t="s">
-        <v>3</v>
-      </c>
-      <c r="H71" s="2">
+      <c r="H71" t="s">
+        <v>3</v>
+      </c>
+      <c r="I71" s="2">
         <v>0.94845085470099999</v>
       </c>
-      <c r="I71" s="2">
+      <c r="J71" s="2">
         <v>0.948387035441</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>12</v>
       </c>
@@ -1352,29 +1427,32 @@
         <v>79</v>
       </c>
       <c r="F75" t="s">
+        <v>96</v>
+      </c>
+      <c r="G75" t="s">
         <v>87</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="H75" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H75" s="2">
+      <c r="I75" s="2">
         <v>0.95576698380900005</v>
       </c>
-      <c r="I75" s="2">
+      <c r="J75" s="2">
         <v>0.95561167305100003</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>76</v>
       </c>
@@ -1388,19 +1466,22 @@
         <v>79</v>
       </c>
       <c r="F78" t="s">
+        <v>96</v>
+      </c>
+      <c r="G78" t="s">
         <v>87</v>
       </c>
-      <c r="G78" s="3" t="s">
+      <c r="H78" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H78" s="2">
+      <c r="I78" s="2">
         <v>0.94658654648600005</v>
       </c>
-      <c r="I78" s="2">
+      <c r="J78" s="2">
         <v>0.94636419618400003</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>13</v>
       </c>
@@ -1408,22 +1489,22 @@
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>14</v>
       </c>
@@ -1440,34 +1521,37 @@
         <v>79</v>
       </c>
       <c r="F83" t="s">
+        <v>96</v>
+      </c>
+      <c r="G83" t="s">
         <v>87</v>
       </c>
-      <c r="G83" s="3" t="s">
+      <c r="H83" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="H83" s="2">
+      <c r="I83" s="2">
         <v>0.94858955099300002</v>
       </c>
-      <c r="I83" s="2">
+      <c r="J83" s="2">
         <v>0.94837828856600004</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>15</v>
       </c>
@@ -1484,34 +1568,37 @@
         <v>79</v>
       </c>
       <c r="F87" t="s">
+        <v>96</v>
+      </c>
+      <c r="G87" t="s">
         <v>87</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>90</v>
       </c>
-      <c r="H87" s="2">
+      <c r="I87" s="2">
         <v>0.95543314972500004</v>
       </c>
-      <c r="I87" s="2">
+      <c r="J87" s="2">
         <v>0.95534929330200002</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>16</v>
       </c>
@@ -1528,34 +1615,37 @@
         <v>79</v>
       </c>
       <c r="F91" t="s">
+        <v>96</v>
+      </c>
+      <c r="G91" t="s">
         <v>87</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>91</v>
       </c>
-      <c r="H91" s="2">
+      <c r="I91" s="2">
         <v>0.92889334001000001</v>
       </c>
-      <c r="I91" s="2">
+      <c r="J91" s="2">
         <v>0.92868399047799999</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>17</v>
       </c>
@@ -1572,37 +1662,227 @@
         <v>79</v>
       </c>
       <c r="F95" t="s">
+        <v>96</v>
+      </c>
+      <c r="G95" t="s">
         <v>87</v>
       </c>
-      <c r="G95" t="s">
-        <v>3</v>
-      </c>
-      <c r="H95" s="2">
+      <c r="H95" t="s">
+        <v>3</v>
+      </c>
+      <c r="I95" s="2">
         <v>0.90233722871499999</v>
       </c>
-      <c r="I95" s="2">
+      <c r="J95" s="2">
         <v>0.90060578603599994</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>98</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98" t="s">
+        <v>79</v>
+      </c>
+      <c r="F98" t="s">
+        <v>94</v>
+      </c>
+      <c r="G98" t="s">
+        <v>97</v>
+      </c>
+      <c r="H98" t="s">
+        <v>3</v>
+      </c>
+      <c r="I98" s="2">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="J98" s="2">
+        <v>0.95244290626100003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>18</v>
       </c>
+      <c r="B99" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>19</v>
+      </c>
+      <c r="B103" t="s">
+        <v>74</v>
+      </c>
+      <c r="C103" t="s">
+        <v>102</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103" t="s">
+        <v>79</v>
+      </c>
+      <c r="F103" t="s">
+        <v>94</v>
+      </c>
+      <c r="G103" t="s">
+        <v>100</v>
+      </c>
+      <c r="H103" t="s">
+        <v>3</v>
+      </c>
+      <c r="I103" s="2">
+        <v>0.94033333333299995</v>
+      </c>
+      <c r="J103" s="2">
+        <v>0.940308845778</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>20</v>
+      </c>
+      <c r="B107" t="s">
+        <v>99</v>
+      </c>
+      <c r="C107" t="s">
+        <v>98</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107" t="s">
+        <v>79</v>
+      </c>
+      <c r="F107" t="s">
+        <v>94</v>
+      </c>
+      <c r="G107" t="s">
+        <v>97</v>
+      </c>
+      <c r="H107" t="s">
+        <v>3</v>
+      </c>
+      <c r="I107" s="2">
+        <v>0.95250000000000001</v>
+      </c>
+      <c r="J107" s="2">
+        <v>0.95244290626100003</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>21</v>
+      </c>
+      <c r="B111" t="s">
+        <v>80</v>
+      </c>
+      <c r="C111" t="s">
+        <v>104</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111" t="s">
+        <v>79</v>
+      </c>
+      <c r="F111" t="s">
+        <v>94</v>
+      </c>
+      <c r="G111" t="s">
+        <v>97</v>
+      </c>
+      <c r="H111" t="s">
+        <v>3</v>
+      </c>
+      <c r="I111" s="2">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="J111" s="2">
+        <v>92.298818414300001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2139,10 +2419,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K156"/>
+  <dimension ref="A1:L184"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView topLeftCell="D148" workbookViewId="0">
+      <selection activeCell="G162" sqref="G162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,12 +2430,12 @@
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="87.42578125" customWidth="1"/>
     <col min="3" max="3" width="71.42578125" customWidth="1"/>
-    <col min="5" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="5" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2163,16 +2443,19 @@
         <v>14980</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>14976</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -2189,22 +2472,25 @@
         <v>58</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2221,77 +2507,80 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
         <v>69</v>
       </c>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
       <c r="H6" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="2">
         <v>0.93057409879800002</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>0.93037252707899998</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2308,77 +2597,80 @@
         <v>17</v>
       </c>
       <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" t="s">
         <v>69</v>
       </c>
-      <c r="G18" t="s">
-        <v>3</v>
-      </c>
       <c r="H18" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="2">
         <v>0.930240320427</v>
       </c>
-      <c r="J18" s="2">
+      <c r="K18" s="2">
         <v>0.93003459602600003</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2395,52 +2687,55 @@
         <v>17</v>
       </c>
       <c r="F30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G30" t="s">
         <v>69</v>
       </c>
-      <c r="G30" t="s">
-        <v>3</v>
-      </c>
       <c r="H30" t="s">
         <v>3</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="2">
         <v>0.93124165554100002</v>
       </c>
-      <c r="J30" s="2">
+      <c r="K30" s="2">
         <v>0.93103573022700004</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2457,52 +2752,55 @@
         <v>17</v>
       </c>
       <c r="F37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" t="s">
         <v>69</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>61</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>1</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>0.93190921228300005</v>
       </c>
-      <c r="J37" s="2">
+      <c r="K37" s="2">
         <v>0.93175335980700003</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5</v>
       </c>
@@ -2519,52 +2817,55 @@
         <v>17</v>
       </c>
       <c r="F44" t="s">
+        <v>96</v>
+      </c>
+      <c r="G44" t="s">
         <v>69</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>61</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="2">
+      <c r="J44" s="2">
         <v>0.93124165554100002</v>
       </c>
-      <c r="J44" s="2">
+      <c r="K44" s="2">
         <v>0.93106654963699997</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2581,52 +2882,55 @@
         <v>17</v>
       </c>
       <c r="F51" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" t="s">
         <v>69</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>61</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
         <v>56</v>
       </c>
-      <c r="I51" s="2">
+      <c r="J51" s="2">
         <v>0.92122830440600001</v>
       </c>
-      <c r="J51" s="2">
+      <c r="K51" s="2">
         <v>0.92100673278</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7</v>
       </c>
@@ -2643,52 +2947,55 @@
         <v>17</v>
       </c>
       <c r="F58" t="s">
+        <v>96</v>
+      </c>
+      <c r="G58" t="s">
         <v>69</v>
       </c>
-      <c r="G58" t="s">
-        <v>3</v>
-      </c>
       <c r="H58" t="s">
         <v>3</v>
       </c>
-      <c r="I58" s="2">
+      <c r="I58" t="s">
+        <v>3</v>
+      </c>
+      <c r="J58" s="2">
         <v>0.92721202003299996</v>
       </c>
-      <c r="J58" s="2">
+      <c r="K58" s="2">
         <v>0.92700255257200004</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>8</v>
       </c>
@@ -2705,52 +3012,55 @@
         <v>17</v>
       </c>
       <c r="F65" t="s">
+        <v>96</v>
+      </c>
+      <c r="G65" t="s">
         <v>69</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>61</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>57</v>
       </c>
-      <c r="I65" s="2">
+      <c r="J65" s="2">
         <v>0.92721202003299996</v>
       </c>
-      <c r="J65" s="2">
+      <c r="K65" s="2">
         <v>0.92702874226999998</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9</v>
       </c>
@@ -2767,52 +3077,55 @@
         <v>17</v>
       </c>
       <c r="F72" t="s">
+        <v>96</v>
+      </c>
+      <c r="G72" t="s">
         <v>69</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>62</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>64</v>
       </c>
-      <c r="I72" s="2">
+      <c r="J72" s="2">
         <v>0.92420701168599995</v>
       </c>
-      <c r="J72" s="2">
+      <c r="K72" s="2">
         <v>0.92395686509399999</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>10</v>
       </c>
@@ -2829,52 +3142,55 @@
         <v>17</v>
       </c>
       <c r="F79" t="s">
+        <v>96</v>
+      </c>
+      <c r="G79" t="s">
         <v>69</v>
       </c>
-      <c r="G79" t="s">
-        <v>3</v>
-      </c>
       <c r="H79" t="s">
         <v>3</v>
       </c>
-      <c r="I79" s="2">
+      <c r="I79" t="s">
+        <v>3</v>
+      </c>
+      <c r="J79" s="2">
         <v>0.92621035058400003</v>
       </c>
-      <c r="J79" s="2">
+      <c r="K79" s="2">
         <v>0.92597375524299996</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>11</v>
       </c>
@@ -2891,53 +3207,56 @@
         <v>17</v>
       </c>
       <c r="F86" t="s">
+        <v>96</v>
+      </c>
+      <c r="G86" t="s">
         <v>69</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>61</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>59</v>
       </c>
-      <c r="I86" s="2">
+      <c r="J86" s="2">
         <v>0.93257676902499997</v>
       </c>
-      <c r="J86" s="2">
+      <c r="K86" s="2">
         <v>0.93241671326499997</v>
       </c>
-      <c r="K86" s="2"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86" s="2"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>12</v>
       </c>
@@ -2954,52 +3273,55 @@
         <v>17</v>
       </c>
       <c r="F93" t="s">
+        <v>96</v>
+      </c>
+      <c r="G93" t="s">
         <v>69</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>62</v>
       </c>
-      <c r="H93" t="s">
+      <c r="I93" t="s">
         <v>63</v>
       </c>
-      <c r="I93" s="2">
+      <c r="J93" s="2">
         <v>0.91619365609299996</v>
       </c>
-      <c r="J93" s="2">
+      <c r="K93" s="2">
         <v>0.91594885467700005</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>13</v>
       </c>
@@ -3016,52 +3338,55 @@
         <v>17</v>
       </c>
       <c r="F100" t="s">
+        <v>96</v>
+      </c>
+      <c r="G100" t="s">
         <v>69</v>
       </c>
-      <c r="G100" t="s">
-        <v>3</v>
-      </c>
       <c r="H100" t="s">
         <v>3</v>
       </c>
-      <c r="I100" s="2">
+      <c r="I100" t="s">
+        <v>3</v>
+      </c>
+      <c r="J100" s="2">
         <v>0.92420701168599995</v>
       </c>
-      <c r="J100" s="2">
+      <c r="K100" s="2">
         <v>0.92388736352699996</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>14</v>
       </c>
@@ -3078,52 +3403,55 @@
         <v>17</v>
       </c>
       <c r="F107" t="s">
+        <v>96</v>
+      </c>
+      <c r="G107" t="s">
         <v>69</v>
       </c>
-      <c r="G107" t="s">
+      <c r="H107" t="s">
         <v>61</v>
       </c>
-      <c r="H107" t="s">
+      <c r="I107" t="s">
         <v>65</v>
       </c>
-      <c r="I107" s="2">
+      <c r="J107" s="2">
         <v>0.92754590984999996</v>
       </c>
-      <c r="J107" s="2">
+      <c r="K107" s="2">
         <v>0.92724857879900002</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>15</v>
       </c>
@@ -3140,52 +3468,55 @@
         <v>17</v>
       </c>
       <c r="F114" t="s">
+        <v>96</v>
+      </c>
+      <c r="G114" t="s">
         <v>69</v>
       </c>
-      <c r="G114" t="s">
+      <c r="H114" t="s">
         <v>62</v>
       </c>
-      <c r="H114" t="s">
+      <c r="I114" t="s">
         <v>66</v>
       </c>
-      <c r="I114" s="2">
+      <c r="J114" s="2">
         <v>0.92754590984999996</v>
       </c>
-      <c r="J114" s="2">
+      <c r="K114" s="2">
         <v>0.92726484287300004</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>16</v>
       </c>
@@ -3202,47 +3533,50 @@
         <v>67</v>
       </c>
       <c r="F121" t="s">
+        <v>96</v>
+      </c>
+      <c r="G121" t="s">
         <v>69</v>
       </c>
-      <c r="G121" t="s">
+      <c r="H121" t="s">
         <v>61</v>
       </c>
-      <c r="H121" t="s">
+      <c r="I121" t="s">
         <v>1</v>
       </c>
-      <c r="I121" s="2">
+      <c r="J121" s="2">
         <v>0.93124165554100002</v>
       </c>
-      <c r="J121" s="2">
+      <c r="K121" s="2">
         <v>0.93106654963699997</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>17</v>
       </c>
@@ -3259,47 +3593,50 @@
         <v>3</v>
       </c>
       <c r="F127" t="s">
+        <v>96</v>
+      </c>
+      <c r="G127" t="s">
         <v>69</v>
       </c>
-      <c r="G127" t="s">
+      <c r="H127" t="s">
         <v>61</v>
       </c>
-      <c r="H127" t="s">
+      <c r="I127" t="s">
         <v>1</v>
       </c>
-      <c r="I127" s="2">
+      <c r="J127" s="2">
         <v>0.93558077436599996</v>
       </c>
-      <c r="J127" s="2">
+      <c r="K127" s="2">
         <v>0.93539079920099999</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>18</v>
       </c>
@@ -3316,47 +3653,50 @@
         <v>3</v>
       </c>
       <c r="F133" t="s">
+        <v>96</v>
+      </c>
+      <c r="G133" t="s">
         <v>70</v>
       </c>
-      <c r="G133" t="s">
+      <c r="H133" t="s">
         <v>61</v>
       </c>
-      <c r="H133" t="s">
+      <c r="I133" t="s">
         <v>1</v>
       </c>
-      <c r="I133" s="2">
+      <c r="J133" s="2">
         <v>0.92677498330700003</v>
       </c>
-      <c r="J133" s="2">
+      <c r="K133" s="2">
         <v>0.92655824004300003</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>19</v>
       </c>
@@ -3373,47 +3713,50 @@
         <v>3</v>
       </c>
       <c r="F139" t="s">
+        <v>96</v>
+      </c>
+      <c r="G139" t="s">
         <v>71</v>
       </c>
-      <c r="G139" t="s">
+      <c r="H139" t="s">
         <v>61</v>
       </c>
-      <c r="H139" t="s">
+      <c r="I139" t="s">
         <v>1</v>
       </c>
-      <c r="I139" s="2">
+      <c r="J139" s="2">
         <v>0.93135683760700005</v>
       </c>
-      <c r="J139" s="2">
+      <c r="K139" s="2">
         <v>0.93114810886300003</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>20</v>
       </c>
@@ -3430,47 +3773,50 @@
         <v>3</v>
       </c>
       <c r="F145" t="s">
+        <v>96</v>
+      </c>
+      <c r="G145" t="s">
         <v>73</v>
       </c>
-      <c r="G145" t="s">
+      <c r="H145" t="s">
         <v>61</v>
       </c>
-      <c r="H145" t="s">
+      <c r="I145" t="s">
         <v>1</v>
       </c>
-      <c r="I145" s="2">
+      <c r="J145" s="2">
         <v>0.93457943925200004</v>
       </c>
-      <c r="J145" s="2">
+      <c r="K145" s="2">
         <v>0.93435051452899998</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>21</v>
       </c>
@@ -3487,44 +3833,307 @@
         <v>3</v>
       </c>
       <c r="F151" t="s">
+        <v>96</v>
+      </c>
+      <c r="G151" t="s">
         <v>72</v>
       </c>
-      <c r="G151" t="s">
+      <c r="H151" t="s">
         <v>61</v>
       </c>
-      <c r="H151" t="s">
+      <c r="I151" t="s">
         <v>1</v>
       </c>
-      <c r="I151" s="2">
+      <c r="J151" s="2">
         <v>0.93368936359599997</v>
       </c>
-      <c r="J151" s="2">
+      <c r="K151" s="2">
         <v>0.93347648280700002</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>22</v>
+      </c>
+      <c r="B157" t="s">
+        <v>51</v>
+      </c>
+      <c r="C157" t="s">
+        <v>3</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157" t="s">
+        <v>3</v>
+      </c>
+      <c r="F157" t="s">
+        <v>94</v>
+      </c>
+      <c r="G157" t="s">
+        <v>69</v>
+      </c>
+      <c r="H157" t="s">
+        <v>61</v>
+      </c>
+      <c r="I157" t="s">
+        <v>1</v>
+      </c>
+      <c r="J157" s="2">
+        <v>0.9395</v>
+      </c>
+      <c r="K157" s="2">
+        <v>0.93943733435400001</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>23</v>
+      </c>
+      <c r="B164" t="s">
+        <v>51</v>
+      </c>
+      <c r="C164" t="s">
+        <v>3</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164" t="s">
+        <v>3</v>
+      </c>
+      <c r="F164" t="s">
+        <v>94</v>
+      </c>
+      <c r="G164" t="s">
+        <v>69</v>
+      </c>
+      <c r="H164" t="s">
+        <v>61</v>
+      </c>
+      <c r="I164" t="s">
+        <v>1</v>
+      </c>
+      <c r="J164" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="K164" s="2">
+        <v>0.93743526276199995</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>24</v>
+      </c>
+      <c r="B171" t="s">
+        <v>51</v>
+      </c>
+      <c r="C171" t="s">
+        <v>3</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171" t="s">
+        <v>3</v>
+      </c>
+      <c r="F171" t="s">
+        <v>94</v>
+      </c>
+      <c r="G171" t="s">
+        <v>70</v>
+      </c>
+      <c r="H171" t="s">
+        <v>61</v>
+      </c>
+      <c r="I171" t="s">
+        <v>1</v>
+      </c>
+      <c r="J171" s="2">
+        <v>0.93566666666700005</v>
+      </c>
+      <c r="K171" s="2">
+        <v>0.93560315519299997</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>25</v>
+      </c>
+      <c r="B178" t="s">
+        <v>51</v>
+      </c>
+      <c r="C178" t="s">
+        <v>3</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178" t="s">
+        <v>3</v>
+      </c>
+      <c r="F178" t="s">
+        <v>94</v>
+      </c>
+      <c r="G178" t="s">
+        <v>69</v>
+      </c>
+      <c r="H178" t="s">
+        <v>61</v>
+      </c>
+      <c r="I178" t="s">
+        <v>3</v>
+      </c>
+      <c r="J178" s="2">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="K178" s="2">
+        <v>0.94189523809499998</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>